<commit_message>
Alterações na Monografia e nas sprints 7 e 8
</commit_message>
<xml_diff>
--- a/Sprints/sprint 1.xlsx
+++ b/Sprints/sprint 1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PIM3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\PIM\Sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC2F388-A68A-4509-86CF-C29C2D5DBCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19665" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sprint 1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>DATA</t>
   </si>
@@ -41,28 +42,25 @@
     <t>20/03/2024 - 27/03/2024</t>
   </si>
   <si>
-    <t>Realizado o Backlog e endereço do Git do projeto</t>
-  </si>
-  <si>
     <t>Grupo</t>
   </si>
   <si>
-    <t>Em processo</t>
-  </si>
-  <si>
-    <t>Crianção de Tela de Login e Recuperação de Senha</t>
-  </si>
-  <si>
     <t>Gabriel</t>
   </si>
   <si>
     <t>Pronto</t>
+  </si>
+  <si>
+    <t>Criação do Backlog e Git do projeto</t>
+  </si>
+  <si>
+    <t>Criação da 1ª versão das telas de Login e Recuperação de Senha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,10 +90,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -103,7 +104,7 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -134,13 +135,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D3" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:D3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:D3" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="DATA" dataDxfId="5"/>
-    <tableColumn id="2" name="TAREFA REALIZADA " dataDxfId="4"/>
-    <tableColumn id="3" name="QUEM REALIZOU" dataDxfId="3"/>
-    <tableColumn id="4" name="STATUS" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="DATA" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TAREFA REALIZADA " dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="QUEM REALIZOU" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="STATUS" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -408,17 +409,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -441,11 +442,11 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -455,14 +456,14 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>